<commit_message>
Cross Browsing and log propertiws file modified
</commit_message>
<xml_diff>
--- a/Input_ExcelSheet/Hospital_Loc.xlsx
+++ b/Input_ExcelSheet/Hospital_Loc.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>City</t>
   </si>
@@ -28,7 +28,10 @@
     <t>Hospital</t>
   </si>
   <si>
-    <t>Chennai</t>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>London</t>
   </si>
 </sst>
 </file>
@@ -364,7 +367,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -388,7 +391,9 @@
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>

</xml_diff>